<commit_message>
adding strain names and updating protocoll
</commit_message>
<xml_diff>
--- a/old_database/crypto/bioSample/bioSample_2002.xlsx
+++ b/old_database/crypto/bioSample/bioSample_2002.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/old_database/crypto/bioSample/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D89D34B2-1057-4C47-BB62-24E5E37076C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="18620" yWindow="680" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="43">
   <si>
     <t>harvestDate</t>
   </si>
@@ -58,9 +64,6 @@
     <t>1.24.17</t>
   </si>
   <si>
-    <t>Retrofitted_2002</t>
-  </si>
-  <si>
     <t>CNAG_00000</t>
   </si>
   <si>
@@ -101,13 +104,58 @@
   </si>
   <si>
     <t>37C.CO2</t>
+  </si>
+  <si>
+    <t>S.GISH</t>
+  </si>
+  <si>
+    <t>90minuteInduction</t>
+  </si>
+  <si>
+    <t>KN99alpha</t>
+  </si>
+  <si>
+    <t>TDY1960</t>
+  </si>
+  <si>
+    <t>TDY1700</t>
+  </si>
+  <si>
+    <t>TDY1936</t>
+  </si>
+  <si>
+    <t>TDY1945</t>
+  </si>
+  <si>
+    <t>TDY1974</t>
+  </si>
+  <si>
+    <t>TDY2004</t>
+  </si>
+  <si>
+    <t>TDY1174</t>
+  </si>
+  <si>
+    <t>TDY1338</t>
+  </si>
+  <si>
+    <t>TDY1948</t>
+  </si>
+  <si>
+    <t>TDY2017</t>
+  </si>
+  <si>
+    <t>TDY1963</t>
+  </si>
+  <si>
+    <t>TDY1981</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,6 +218,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -216,7 +272,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -248,9 +304,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -282,6 +356,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -457,14 +549,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:F4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -502,21 +596,27 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" t="s">
+        <v>30</v>
+      </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K2">
         <v>90</v>
@@ -525,21 +625,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" t="s">
+        <v>30</v>
+      </c>
       <c r="G3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K3">
         <v>90</v>
@@ -548,21 +654,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" t="s">
+        <v>30</v>
+      </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K4">
         <v>90</v>
@@ -571,21 +683,27 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" t="s">
+        <v>31</v>
+      </c>
       <c r="G5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K5">
         <v>90</v>
@@ -594,21 +712,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" t="s">
+        <v>31</v>
+      </c>
       <c r="G6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K6">
         <v>90</v>
@@ -617,21 +741,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" t="s">
+        <v>31</v>
+      </c>
       <c r="G7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K7">
         <v>90</v>
@@ -640,21 +770,27 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C8">
         <v>7</v>
       </c>
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" t="s">
+        <v>32</v>
+      </c>
       <c r="G8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K8">
         <v>90</v>
@@ -663,21 +799,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C9">
         <v>8</v>
       </c>
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" t="s">
+        <v>32</v>
+      </c>
       <c r="G9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K9">
         <v>90</v>
@@ -686,21 +828,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C10">
         <v>9</v>
       </c>
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" t="s">
+        <v>32</v>
+      </c>
       <c r="G10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K10">
         <v>90</v>
@@ -709,21 +857,27 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C11">
         <v>10</v>
       </c>
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" t="s">
+        <v>33</v>
+      </c>
       <c r="G11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K11">
         <v>90</v>
@@ -732,21 +886,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C12">
         <v>11</v>
       </c>
+      <c r="D12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" t="s">
+        <v>33</v>
+      </c>
       <c r="G12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K12">
         <v>90</v>
@@ -755,21 +915,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C13">
         <v>12</v>
       </c>
+      <c r="D13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" t="s">
+        <v>33</v>
+      </c>
       <c r="G13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K13">
         <v>90</v>
@@ -778,21 +944,27 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C14">
         <v>13</v>
       </c>
+      <c r="D14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" t="s">
+        <v>34</v>
+      </c>
       <c r="G14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K14">
         <v>90</v>
@@ -801,21 +973,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C15">
         <v>14</v>
       </c>
+      <c r="D15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" t="s">
+        <v>34</v>
+      </c>
       <c r="G15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K15">
         <v>90</v>
@@ -824,21 +1002,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C16">
         <v>15</v>
       </c>
+      <c r="D16" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" t="s">
+        <v>34</v>
+      </c>
       <c r="G16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K16">
         <v>90</v>
@@ -847,21 +1031,27 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C17">
         <v>16</v>
       </c>
+      <c r="D17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" t="s">
+        <v>35</v>
+      </c>
       <c r="G17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K17">
         <v>90</v>
@@ -870,21 +1060,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C18">
         <v>17</v>
       </c>
+      <c r="D18" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" t="s">
+        <v>35</v>
+      </c>
       <c r="G18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K18">
         <v>90</v>
@@ -893,21 +1089,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C19">
         <v>18</v>
       </c>
+      <c r="D19" t="s">
+        <v>29</v>
+      </c>
+      <c r="F19" t="s">
+        <v>35</v>
+      </c>
       <c r="G19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K19">
         <v>90</v>
@@ -916,21 +1118,27 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C20">
         <v>19</v>
       </c>
+      <c r="D20" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" t="s">
+        <v>36</v>
+      </c>
       <c r="G20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K20">
         <v>90</v>
@@ -939,21 +1147,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>12</v>
       </c>
       <c r="B21" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C21">
         <v>20</v>
       </c>
+      <c r="D21" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21" t="s">
+        <v>36</v>
+      </c>
       <c r="G21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K21">
         <v>90</v>
@@ -962,21 +1176,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>12</v>
       </c>
       <c r="B22" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C22">
         <v>21</v>
       </c>
+      <c r="D22" t="s">
+        <v>29</v>
+      </c>
+      <c r="F22" t="s">
+        <v>36</v>
+      </c>
       <c r="G22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K22">
         <v>90</v>
@@ -985,21 +1205,27 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>13</v>
       </c>
       <c r="B23" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C23">
         <v>22</v>
       </c>
+      <c r="D23" t="s">
+        <v>29</v>
+      </c>
+      <c r="F23" t="s">
+        <v>30</v>
+      </c>
       <c r="G23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K23">
         <v>90</v>
@@ -1008,21 +1234,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>13</v>
       </c>
       <c r="B24" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C24">
         <v>23</v>
       </c>
+      <c r="D24" t="s">
+        <v>29</v>
+      </c>
+      <c r="F24" t="s">
+        <v>30</v>
+      </c>
       <c r="G24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K24">
         <v>90</v>
@@ -1031,21 +1263,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>13</v>
       </c>
       <c r="B25" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C25">
         <v>24</v>
       </c>
+      <c r="D25" t="s">
+        <v>29</v>
+      </c>
+      <c r="F25" t="s">
+        <v>30</v>
+      </c>
       <c r="G25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K25">
         <v>90</v>
@@ -1054,21 +1292,27 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>13</v>
       </c>
       <c r="B26" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C26">
         <v>25</v>
       </c>
+      <c r="D26" t="s">
+        <v>29</v>
+      </c>
+      <c r="F26" t="s">
+        <v>40</v>
+      </c>
       <c r="G26" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K26">
         <v>90</v>
@@ -1077,21 +1321,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>13</v>
       </c>
       <c r="B27" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C27">
         <v>26</v>
       </c>
+      <c r="D27" t="s">
+        <v>29</v>
+      </c>
+      <c r="F27" t="s">
+        <v>40</v>
+      </c>
       <c r="G27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K27">
         <v>90</v>
@@ -1100,21 +1350,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>13</v>
       </c>
       <c r="B28" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C28">
         <v>27</v>
       </c>
+      <c r="D28" t="s">
+        <v>29</v>
+      </c>
+      <c r="F28" t="s">
+        <v>40</v>
+      </c>
       <c r="G28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K28">
         <v>90</v>
@@ -1123,21 +1379,27 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>13</v>
       </c>
       <c r="B29" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C29">
         <v>28</v>
       </c>
+      <c r="D29" t="s">
+        <v>29</v>
+      </c>
+      <c r="F29" t="s">
+        <v>41</v>
+      </c>
       <c r="G29" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K29">
         <v>90</v>
@@ -1146,21 +1408,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>13</v>
       </c>
       <c r="B30" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C30">
         <v>29</v>
       </c>
+      <c r="D30" t="s">
+        <v>29</v>
+      </c>
+      <c r="F30" t="s">
+        <v>41</v>
+      </c>
       <c r="G30" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K30">
         <v>90</v>
@@ -1169,21 +1437,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>13</v>
       </c>
       <c r="B31" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C31">
         <v>30</v>
       </c>
+      <c r="D31" t="s">
+        <v>29</v>
+      </c>
+      <c r="F31" t="s">
+        <v>41</v>
+      </c>
       <c r="G31" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K31">
         <v>90</v>
@@ -1192,21 +1466,27 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>13</v>
       </c>
       <c r="B32" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C32">
         <v>31</v>
       </c>
+      <c r="D32" t="s">
+        <v>29</v>
+      </c>
+      <c r="F32" t="s">
+        <v>33</v>
+      </c>
       <c r="G32" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K32">
         <v>90</v>
@@ -1215,21 +1495,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>13</v>
       </c>
       <c r="B33" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C33">
         <v>32</v>
       </c>
+      <c r="D33" t="s">
+        <v>29</v>
+      </c>
+      <c r="F33" t="s">
+        <v>33</v>
+      </c>
       <c r="G33" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J33" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K33">
         <v>90</v>
@@ -1238,21 +1524,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>13</v>
       </c>
       <c r="B34" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C34">
         <v>33</v>
       </c>
+      <c r="D34" t="s">
+        <v>29</v>
+      </c>
+      <c r="F34" t="s">
+        <v>33</v>
+      </c>
       <c r="G34" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J34" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K34">
         <v>90</v>
@@ -1261,21 +1553,27 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>13</v>
       </c>
       <c r="B35" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C35">
         <v>34</v>
       </c>
+      <c r="D35" t="s">
+        <v>29</v>
+      </c>
+      <c r="F35" t="s">
+        <v>37</v>
+      </c>
       <c r="G35" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J35" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K35">
         <v>90</v>
@@ -1284,21 +1582,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>13</v>
       </c>
       <c r="B36" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C36">
         <v>35</v>
       </c>
+      <c r="D36" t="s">
+        <v>29</v>
+      </c>
+      <c r="F36" t="s">
+        <v>37</v>
+      </c>
       <c r="G36" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J36" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K36">
         <v>90</v>
@@ -1307,21 +1611,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>13</v>
       </c>
       <c r="B37" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C37">
         <v>36</v>
       </c>
+      <c r="D37" t="s">
+        <v>29</v>
+      </c>
+      <c r="F37" t="s">
+        <v>37</v>
+      </c>
       <c r="G37" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J37" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K37">
         <v>90</v>
@@ -1330,21 +1640,27 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>13</v>
       </c>
       <c r="B38" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C38">
         <v>37</v>
       </c>
+      <c r="D38" t="s">
+        <v>29</v>
+      </c>
+      <c r="F38" t="s">
+        <v>38</v>
+      </c>
       <c r="G38" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J38" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K38">
         <v>90</v>
@@ -1353,21 +1669,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>13</v>
       </c>
       <c r="B39" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C39">
         <v>38</v>
       </c>
+      <c r="D39" t="s">
+        <v>29</v>
+      </c>
+      <c r="F39" t="s">
+        <v>38</v>
+      </c>
       <c r="G39" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J39" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K39">
         <v>90</v>
@@ -1376,21 +1698,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>13</v>
       </c>
       <c r="B40" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C40">
         <v>39</v>
       </c>
+      <c r="D40" t="s">
+        <v>29</v>
+      </c>
+      <c r="F40" t="s">
+        <v>38</v>
+      </c>
       <c r="G40" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J40" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K40">
         <v>90</v>
@@ -1399,21 +1727,27 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>13</v>
       </c>
       <c r="B41" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C41">
         <v>40</v>
       </c>
+      <c r="D41" t="s">
+        <v>29</v>
+      </c>
+      <c r="F41" t="s">
+        <v>35</v>
+      </c>
       <c r="G41" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J41" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K41">
         <v>90</v>
@@ -1422,21 +1756,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>13</v>
       </c>
       <c r="B42" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C42">
         <v>41</v>
       </c>
+      <c r="D42" t="s">
+        <v>29</v>
+      </c>
+      <c r="F42" t="s">
+        <v>35</v>
+      </c>
       <c r="G42" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J42" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K42">
         <v>90</v>
@@ -1445,21 +1785,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:12">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>13</v>
       </c>
       <c r="B43" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C43">
         <v>42</v>
       </c>
+      <c r="D43" t="s">
+        <v>29</v>
+      </c>
+      <c r="F43" t="s">
+        <v>35</v>
+      </c>
       <c r="G43" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J43" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K43">
         <v>90</v>
@@ -1468,21 +1814,27 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:12">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>13</v>
       </c>
       <c r="B44" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C44">
         <v>43</v>
       </c>
+      <c r="D44" t="s">
+        <v>29</v>
+      </c>
+      <c r="F44" t="s">
+        <v>39</v>
+      </c>
       <c r="G44" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J44" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K44">
         <v>90</v>
@@ -1491,21 +1843,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:12">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>13</v>
       </c>
       <c r="B45" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C45">
         <v>44</v>
       </c>
+      <c r="D45" t="s">
+        <v>29</v>
+      </c>
+      <c r="F45" t="s">
+        <v>39</v>
+      </c>
       <c r="G45" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J45" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K45">
         <v>90</v>
@@ -1514,21 +1872,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:12">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>13</v>
       </c>
       <c r="B46" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C46">
         <v>45</v>
       </c>
+      <c r="D46" t="s">
+        <v>29</v>
+      </c>
+      <c r="F46" t="s">
+        <v>39</v>
+      </c>
       <c r="G46" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J46" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K46">
         <v>90</v>
@@ -1537,21 +1901,27 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:12">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>13</v>
       </c>
       <c r="B47" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C47">
         <v>46</v>
       </c>
+      <c r="D47" t="s">
+        <v>29</v>
+      </c>
+      <c r="F47" t="s">
+        <v>42</v>
+      </c>
       <c r="G47" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J47" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K47">
         <v>90</v>
@@ -1560,21 +1930,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:12">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>13</v>
       </c>
       <c r="B48" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C48">
         <v>47</v>
       </c>
+      <c r="D48" t="s">
+        <v>29</v>
+      </c>
+      <c r="F48" t="s">
+        <v>42</v>
+      </c>
       <c r="G48" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K48">
         <v>90</v>
@@ -1583,21 +1959,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:12">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>13</v>
       </c>
       <c r="B49" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C49">
         <v>48</v>
       </c>
+      <c r="D49" t="s">
+        <v>29</v>
+      </c>
+      <c r="F49" t="s">
+        <v>42</v>
+      </c>
       <c r="G49" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J49" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K49">
         <v>90</v>

</xml_diff>